<commit_message>
better ref for swimming crab in demak
</commit_message>
<xml_diff>
--- a/R/data/Indonesia Life History Database.xlsx
+++ b/R/data/Indonesia Life History Database.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmcdonald/github/afamAppPackage/R/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmcdonald/github/afamAppPackage/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="33340" windowHeight="19520" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="559">
   <si>
     <t>General Information</t>
   </si>
@@ -1328,12 +1328,6 @@
     <t>Australia</t>
   </si>
   <si>
-    <t>Carapace width. Derived from size-frequency data from Cockburn Sound, Australia.</t>
-  </si>
-  <si>
-    <t>Derived from size-frequency data from Cockburn Sound, Australia.</t>
-  </si>
-  <si>
     <t>India. Calculated by Dineshbabu et al. using Srinath's (1990) empirical equation.</t>
   </si>
   <si>
@@ -1347,9 +1341,6 @@
   </si>
   <si>
     <t>Kangas MI (2000) Synopsis of the biology and exploitation of the blue swimmer crab, Portunus pelagicus Linnaeus, in Western Australia. Fisheries Research Division, Western Australia. Fisheries Research Report 121, 1-22.</t>
-  </si>
-  <si>
-    <t>de Lestang S, NG Hall, &amp; IC Potter (2003) Do the age compositions and growth of the crab Portunus pelagicus in marine embayments and estuaries differ? Journal of the Marine Biological Association of the United Kingdom, 83, 971-978.</t>
   </si>
   <si>
     <t>Dineshbabu AP, B Shridhara, &amp; Y Muniyappa (2008) Biology and exploitation of the blue swimmer crab, Portunus pelagicus, from south Karnataka coast, India. Indian J. Fish., 55(3), 215-220.</t>
@@ -1758,6 +1749,12 @@
   <si>
     <t>Newman, S.J., 2002. Growth rate, age determination, natural mortality and production potential of the scarlet seaperch, Lutjanus malabaricus Schneider 1801, off the Pilbara coast of north-western Australia. Fish. Res. 58, 215–225. doi:10.1016/S0165-7836(01)00367-8</t>
   </si>
+  <si>
+    <t xml:space="preserve">Pamungkas, Aditya Sinugraha, Zairion, and Kamal, M Mukhlis. Kajian Stok Rajungan (Portunus pelagicus) dengan Analisis Frekuensi Ukuran di Perairan Pesisir Lampung Timur. http://repository.ipb.ac.id/handle/123456789/64573. 2013. </t>
+  </si>
+  <si>
+    <t>Study from East Lampung, Indonesia</t>
+  </si>
 </sst>
 </file>
 
@@ -2135,48 +2132,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2190,6 +2148,45 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2497,8 +2494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO970"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20:G20"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2544,7 +2541,7 @@
       <c r="K1" s="49"/>
       <c r="L1" s="49"/>
       <c r="M1" s="48" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="N1" s="48"/>
       <c r="O1" s="48"/>
@@ -2810,17 +2807,17 @@
         <v>42</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="38" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="22"/>
@@ -2963,14 +2960,14 @@
         <v>43</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="38" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="H7" s="42"/>
       <c r="I7" s="22"/>
@@ -3108,17 +3105,17 @@
         <v>42</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="38" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="H9" s="42"/>
       <c r="I9" s="43"/>
@@ -3876,17 +3873,17 @@
         <v>42</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="38" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
@@ -3945,17 +3942,17 @@
         <v>42</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="38" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="H20" s="22"/>
       <c r="I20" s="22"/>
@@ -4591,13 +4588,13 @@
         <v>135</v>
       </c>
       <c r="M28" s="24">
-        <v>15.27</v>
+        <v>19.16</v>
       </c>
       <c r="N28" s="24">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="O28" s="24">
-        <v>-0.56999999999999995</v>
+        <v>-7.2800000000000004E-2</v>
       </c>
       <c r="P28" s="24">
         <v>2.2000000000000002</v>
@@ -4879,17 +4876,17 @@
         <v>42</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F32" s="20"/>
       <c r="G32" s="38" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="H32" s="42"/>
       <c r="I32" s="22"/>
@@ -40103,8 +40100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI693"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P30" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -40134,17 +40131,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
       <c r="H1" s="49" t="s">
         <v>1</v>
       </c>
@@ -40153,7 +40150,7 @@
       <c r="K1" s="49"/>
       <c r="L1" s="49"/>
       <c r="M1" s="48" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="N1" s="48"/>
       <c r="O1" s="48"/>
@@ -40179,7 +40176,7 @@
       <c r="AI1" s="5"/>
     </row>
     <row r="2" spans="1:35" s="13" customFormat="1" ht="39" x14ac:dyDescent="0.2">
-      <c r="A2" s="60"/>
+      <c r="A2" s="67"/>
       <c r="B2" s="15" t="s">
         <v>198</v>
       </c>
@@ -40257,19 +40254,19 @@
       <c r="A3" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="54" t="s">
+      <c r="B3" s="63"/>
+      <c r="C3" s="64" t="s">
+        <v>542</v>
+      </c>
+      <c r="D3" s="65" t="s">
+        <v>547</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>546</v>
+      </c>
+      <c r="F3" s="54"/>
+      <c r="G3" s="53" t="s">
         <v>545</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>550</v>
-      </c>
-      <c r="E3" s="56" t="s">
-        <v>549</v>
-      </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="56" t="s">
-        <v>548</v>
       </c>
       <c r="H3" s="31"/>
       <c r="I3" s="31"/>
@@ -40304,37 +40301,37 @@
       <c r="A4" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="56"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="53"/>
       <c r="H4" s="25"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
       <c r="K4" s="25"/>
       <c r="L4" s="32"/>
       <c r="M4" s="33" t="s">
+        <v>548</v>
+      </c>
+      <c r="N4" s="33" t="s">
+        <v>548</v>
+      </c>
+      <c r="O4" s="33" t="s">
+        <v>548</v>
+      </c>
+      <c r="P4" s="33" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q4" s="33" t="s">
+        <v>550</v>
+      </c>
+      <c r="R4" s="33" t="s">
+        <v>550</v>
+      </c>
+      <c r="S4" s="33" t="s">
         <v>551</v>
-      </c>
-      <c r="N4" s="33" t="s">
-        <v>551</v>
-      </c>
-      <c r="O4" s="33" t="s">
-        <v>551</v>
-      </c>
-      <c r="P4" s="33" t="s">
-        <v>552</v>
-      </c>
-      <c r="Q4" s="33" t="s">
-        <v>553</v>
-      </c>
-      <c r="R4" s="33" t="s">
-        <v>553</v>
-      </c>
-      <c r="S4" s="33" t="s">
-        <v>554</v>
       </c>
       <c r="T4" s="33" t="s">
         <v>219</v>
@@ -40359,20 +40356,20 @@
       <c r="A5" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="57"/>
-      <c r="G5" s="56" t="s">
+      <c r="F5" s="54"/>
+      <c r="G5" s="53" t="s">
         <v>46</v>
       </c>
       <c r="H5" s="31" t="s">
@@ -40434,12 +40431,12 @@
       <c r="A6" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="56"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="53"/>
       <c r="H6" s="25" t="s">
         <v>213</v>
       </c>
@@ -40499,21 +40496,21 @@
       <c r="A7" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B7" s="53" t="s">
+      <c r="B7" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="64" t="s">
-        <v>514</v>
-      </c>
-      <c r="E7" s="62" t="s">
-        <v>515</v>
-      </c>
-      <c r="F7" s="66"/>
-      <c r="G7" s="62" t="s">
-        <v>516</v>
+      <c r="D7" s="70" t="s">
+        <v>511</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>512</v>
+      </c>
+      <c r="F7" s="61"/>
+      <c r="G7" s="59" t="s">
+        <v>513</v>
       </c>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
@@ -40548,37 +40545,37 @@
       <c r="A8" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="63"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="60"/>
       <c r="H8" s="25"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
       <c r="L8" s="32"/>
       <c r="M8" s="33" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="N8" s="33" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="O8" s="33" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="P8" s="33" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="Q8" s="33" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="R8" s="33" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="S8" s="33" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="T8" s="33" t="s">
         <v>219</v>
@@ -40603,20 +40600,20 @@
       <c r="A9" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="64" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="55" t="s">
+      <c r="D9" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="57"/>
-      <c r="G9" s="56" t="s">
+      <c r="F9" s="54"/>
+      <c r="G9" s="53" t="s">
         <v>51</v>
       </c>
       <c r="H9" s="31" t="s">
@@ -40678,12 +40675,12 @@
       <c r="A10" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="56"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="54"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="25" t="s">
         <v>213</v>
       </c>
@@ -40743,21 +40740,21 @@
       <c r="A11" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="54" t="s">
+      <c r="C11" s="64" t="s">
+        <v>524</v>
+      </c>
+      <c r="D11" s="65" t="s">
+        <v>529</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>528</v>
+      </c>
+      <c r="F11" s="54"/>
+      <c r="G11" s="53" t="s">
         <v>527</v>
-      </c>
-      <c r="D11" s="55" t="s">
-        <v>532</v>
-      </c>
-      <c r="E11" s="56" t="s">
-        <v>531</v>
-      </c>
-      <c r="F11" s="57"/>
-      <c r="G11" s="56" t="s">
-        <v>530</v>
       </c>
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
@@ -40792,37 +40789,37 @@
       <c r="A12" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="56"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="54"/>
+      <c r="G12" s="53"/>
       <c r="H12" s="25"/>
       <c r="I12" s="25"/>
       <c r="J12" s="25"/>
       <c r="K12" s="32"/>
       <c r="L12" s="25"/>
       <c r="M12" s="33" t="s">
+        <v>530</v>
+      </c>
+      <c r="N12" s="36" t="s">
+        <v>530</v>
+      </c>
+      <c r="O12" s="36" t="s">
+        <v>530</v>
+      </c>
+      <c r="P12" s="36" t="s">
+        <v>531</v>
+      </c>
+      <c r="Q12" s="33" t="s">
+        <v>532</v>
+      </c>
+      <c r="R12" s="33" t="s">
+        <v>532</v>
+      </c>
+      <c r="S12" s="36" t="s">
         <v>533</v>
-      </c>
-      <c r="N12" s="36" t="s">
-        <v>533</v>
-      </c>
-      <c r="O12" s="36" t="s">
-        <v>533</v>
-      </c>
-      <c r="P12" s="36" t="s">
-        <v>534</v>
-      </c>
-      <c r="Q12" s="33" t="s">
-        <v>535</v>
-      </c>
-      <c r="R12" s="33" t="s">
-        <v>535</v>
-      </c>
-      <c r="S12" s="36" t="s">
-        <v>536</v>
       </c>
       <c r="T12" s="33" t="s">
         <v>219</v>
@@ -40847,18 +40844,18 @@
       <c r="A13" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="53" t="s">
+      <c r="B13" s="54"/>
+      <c r="C13" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="56" t="s">
+      <c r="E13" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="57"/>
-      <c r="G13" s="53" t="s">
+      <c r="F13" s="54"/>
+      <c r="G13" s="63" t="s">
         <v>56</v>
       </c>
       <c r="H13" s="31" t="s">
@@ -40920,12 +40917,12 @@
       <c r="A14" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="53"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="63"/>
       <c r="H14" s="25" t="s">
         <v>213</v>
       </c>
@@ -40985,20 +40982,20 @@
       <c r="A15" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="53" t="s">
+      <c r="C15" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="E15" s="53" t="s">
+      <c r="E15" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="53" t="s">
+      <c r="F15" s="54"/>
+      <c r="G15" s="63" t="s">
         <v>61</v>
       </c>
       <c r="H15" s="31" t="s">
@@ -41060,12 +41057,12 @@
       <c r="A16" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B16" s="53"/>
-      <c r="C16" s="53"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="53"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="54"/>
+      <c r="G16" s="63"/>
       <c r="H16" s="25" t="s">
         <v>213</v>
       </c>
@@ -41125,18 +41122,18 @@
       <c r="A17" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="53" t="s">
+      <c r="B17" s="54"/>
+      <c r="C17" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="D17" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="53" t="s">
+      <c r="F17" s="54"/>
+      <c r="G17" s="63" t="s">
         <v>65</v>
       </c>
       <c r="H17" s="31" t="s">
@@ -41198,12 +41195,12 @@
       <c r="A18" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="53"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="63"/>
       <c r="H18" s="25" t="s">
         <v>213</v>
       </c>
@@ -41263,18 +41260,18 @@
       <c r="A19" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="53" t="s">
+      <c r="B19" s="54"/>
+      <c r="C19" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="58" t="s">
+      <c r="D19" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="56" t="s">
+      <c r="E19" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="53" t="s">
+      <c r="F19" s="54"/>
+      <c r="G19" s="63" t="s">
         <v>69</v>
       </c>
       <c r="H19" s="31" t="s">
@@ -41336,12 +41333,12 @@
       <c r="A20" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="53"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="63"/>
       <c r="H20" s="25" t="s">
         <v>213</v>
       </c>
@@ -41401,20 +41398,20 @@
       <c r="A21" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B21" s="56" t="s">
+      <c r="B21" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="58" t="s">
+      <c r="D21" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="53" t="s">
+      <c r="E21" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="53" t="s">
+      <c r="F21" s="54"/>
+      <c r="G21" s="63" t="s">
         <v>73</v>
       </c>
       <c r="H21" s="31" t="s">
@@ -41476,12 +41473,12 @@
       <c r="A22" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B22" s="56"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="53"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="63"/>
       <c r="H22" s="25" t="s">
         <v>213</v>
       </c>
@@ -41541,18 +41538,18 @@
       <c r="A23" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="53" t="s">
+      <c r="B23" s="54"/>
+      <c r="C23" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="58" t="s">
+      <c r="D23" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="E23" s="56" t="s">
+      <c r="E23" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="57"/>
-      <c r="G23" s="53" t="s">
+      <c r="F23" s="54"/>
+      <c r="G23" s="63" t="s">
         <v>77</v>
       </c>
       <c r="H23" s="31" t="s">
@@ -41614,12 +41611,12 @@
       <c r="A24" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B24" s="57"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="53"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="63"/>
       <c r="H24" s="25" t="s">
         <v>213</v>
       </c>
@@ -41679,18 +41676,18 @@
       <c r="A25" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="53" t="s">
+      <c r="B25" s="54"/>
+      <c r="C25" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="58" t="s">
+      <c r="D25" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="57"/>
-      <c r="G25" s="53" t="s">
+      <c r="F25" s="54"/>
+      <c r="G25" s="63" t="s">
         <v>81</v>
       </c>
       <c r="H25" s="31" t="s">
@@ -41752,12 +41749,12 @@
       <c r="A26" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="53"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="63"/>
       <c r="H26" s="25" t="s">
         <v>213</v>
       </c>
@@ -41817,20 +41814,20 @@
       <c r="A27" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="58" t="s">
+      <c r="D27" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="53" t="s">
+      <c r="E27" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="F27" s="57"/>
-      <c r="G27" s="53" t="s">
+      <c r="F27" s="54"/>
+      <c r="G27" s="63" t="s">
         <v>85</v>
       </c>
       <c r="H27" s="31" t="s">
@@ -41892,12 +41889,12 @@
       <c r="A28" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="53"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="63"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="63"/>
       <c r="H28" s="25" t="s">
         <v>213</v>
       </c>
@@ -41957,18 +41954,18 @@
       <c r="A29" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B29" s="57"/>
-      <c r="C29" s="53" t="s">
+      <c r="B29" s="54"/>
+      <c r="C29" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="58" t="s">
+      <c r="D29" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="56" t="s">
+      <c r="E29" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="57"/>
-      <c r="G29" s="53" t="s">
+      <c r="F29" s="54"/>
+      <c r="G29" s="63" t="s">
         <v>89</v>
       </c>
       <c r="H29" s="31" t="s">
@@ -42030,12 +42027,12 @@
       <c r="A30" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B30" s="57"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="53"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="63"/>
       <c r="H30" s="25" t="s">
         <v>213</v>
       </c>
@@ -42095,19 +42092,19 @@
       <c r="A31" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="68" t="s">
+      <c r="B31" s="54"/>
+      <c r="C31" s="55" t="s">
+        <v>516</v>
+      </c>
+      <c r="D31" s="57" t="s">
+        <v>521</v>
+      </c>
+      <c r="E31" s="59" t="s">
+        <v>520</v>
+      </c>
+      <c r="F31" s="61"/>
+      <c r="G31" s="55" t="s">
         <v>519</v>
-      </c>
-      <c r="D31" s="70" t="s">
-        <v>524</v>
-      </c>
-      <c r="E31" s="62" t="s">
-        <v>523</v>
-      </c>
-      <c r="F31" s="66"/>
-      <c r="G31" s="68" t="s">
-        <v>522</v>
       </c>
       <c r="H31" s="31"/>
       <c r="I31" s="31"/>
@@ -42142,37 +42139,37 @@
       <c r="A32" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B32" s="57"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="71"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="69"/>
+      <c r="B32" s="54"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="56"/>
       <c r="H32" s="25"/>
       <c r="I32" s="25"/>
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
       <c r="L32" s="25"/>
       <c r="M32" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="N32" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="O32" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="P32" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="Q32" s="33" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="R32" s="33" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="S32" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="T32" s="33" t="s">
         <v>219</v>
@@ -42197,19 +42194,19 @@
       <c r="A33" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B33" s="57"/>
-      <c r="C33" s="68" t="s">
-        <v>519</v>
-      </c>
-      <c r="D33" s="70" t="s">
+      <c r="B33" s="54"/>
+      <c r="C33" s="55" t="s">
+        <v>516</v>
+      </c>
+      <c r="D33" s="57" t="s">
+        <v>552</v>
+      </c>
+      <c r="E33" s="59" t="s">
         <v>555</v>
       </c>
-      <c r="E33" s="62" t="s">
-        <v>558</v>
-      </c>
-      <c r="F33" s="66"/>
-      <c r="G33" s="68" t="s">
-        <v>557</v>
+      <c r="F33" s="61"/>
+      <c r="G33" s="55" t="s">
+        <v>554</v>
       </c>
       <c r="H33" s="31"/>
       <c r="I33" s="31"/>
@@ -42244,37 +42241,37 @@
       <c r="A34" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B34" s="57"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="69"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="56"/>
       <c r="H34" s="25"/>
       <c r="I34" s="25"/>
       <c r="J34" s="25"/>
       <c r="K34" s="25"/>
       <c r="L34" s="25"/>
       <c r="M34" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="N34" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="O34" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="P34" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="Q34" s="33" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="R34" s="33" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="S34" s="33" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="T34" s="33" t="s">
         <v>219</v>
@@ -42299,20 +42296,20 @@
       <c r="A35" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B35" s="54" t="s">
+      <c r="B35" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="53" t="s">
+      <c r="C35" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="59" t="s">
+      <c r="D35" s="69" t="s">
         <v>92</v>
       </c>
-      <c r="E35" s="53" t="s">
+      <c r="E35" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="F35" s="57"/>
-      <c r="G35" s="54" t="s">
+      <c r="F35" s="54"/>
+      <c r="G35" s="64" t="s">
         <v>94</v>
       </c>
       <c r="H35" s="31" t="s">
@@ -42374,12 +42371,12 @@
       <c r="A36" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="53"/>
-      <c r="F36" s="57"/>
-      <c r="G36" s="54"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="64"/>
       <c r="H36" s="25" t="s">
         <v>249</v>
       </c>
@@ -42439,20 +42436,20 @@
       <c r="A37" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="53" t="s">
+      <c r="C37" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="59" t="s">
+      <c r="D37" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="53" t="s">
+      <c r="E37" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="F37" s="57"/>
-      <c r="G37" s="54" t="s">
+      <c r="F37" s="54"/>
+      <c r="G37" s="64" t="s">
         <v>104</v>
       </c>
       <c r="H37" s="31" t="s">
@@ -42514,12 +42511,12 @@
       <c r="A38" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B38" s="54"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="57"/>
-      <c r="G38" s="54"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="69"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="64"/>
       <c r="H38" s="25" t="s">
         <v>249</v>
       </c>
@@ -42579,20 +42576,20 @@
       <c r="A39" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B39" s="54" t="s">
+      <c r="B39" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="53" t="s">
+      <c r="C39" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="E39" s="53" t="s">
+      <c r="E39" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="F39" s="57"/>
-      <c r="G39" s="54" t="s">
+      <c r="F39" s="54"/>
+      <c r="G39" s="64" t="s">
         <v>112</v>
       </c>
       <c r="H39" s="31" t="s">
@@ -42654,12 +42651,12 @@
       <c r="A40" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B40" s="54"/>
-      <c r="C40" s="53"/>
-      <c r="D40" s="59"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="57"/>
-      <c r="G40" s="54"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="64"/>
       <c r="H40" s="25" t="s">
         <v>249</v>
       </c>
@@ -42719,20 +42716,20 @@
       <c r="A41" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="53" t="s">
+      <c r="C41" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="58" t="s">
+      <c r="D41" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="56" t="s">
+      <c r="E41" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="F41" s="57"/>
-      <c r="G41" s="53" t="s">
+      <c r="F41" s="54"/>
+      <c r="G41" s="63" t="s">
         <v>117</v>
       </c>
       <c r="H41" s="31" t="s">
@@ -42794,12 +42791,12 @@
       <c r="A42" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B42" s="56"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="57"/>
-      <c r="G42" s="53"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="63"/>
       <c r="H42" s="25" t="s">
         <v>213</v>
       </c>
@@ -42859,18 +42856,18 @@
       <c r="A43" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B43" s="57"/>
-      <c r="C43" s="53" t="s">
+      <c r="B43" s="54"/>
+      <c r="C43" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="58" t="s">
+      <c r="D43" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="E43" s="56" t="s">
+      <c r="E43" s="53" t="s">
         <v>119</v>
       </c>
-      <c r="F43" s="57"/>
-      <c r="G43" s="53" t="s">
+      <c r="F43" s="54"/>
+      <c r="G43" s="63" t="s">
         <v>120</v>
       </c>
       <c r="H43" s="31" t="s">
@@ -42932,12 +42929,12 @@
       <c r="A44" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B44" s="57"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="58"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="57"/>
-      <c r="G44" s="53"/>
+      <c r="B44" s="54"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="53"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="63"/>
       <c r="H44" s="25" t="s">
         <v>213</v>
       </c>
@@ -42997,20 +42994,20 @@
       <c r="A45" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B45" s="54" t="s">
+      <c r="B45" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="53" t="s">
+      <c r="C45" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="58" t="s">
+      <c r="D45" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="E45" s="53" t="s">
+      <c r="E45" s="63" t="s">
         <v>123</v>
       </c>
-      <c r="F45" s="57"/>
-      <c r="G45" s="54" t="s">
+      <c r="F45" s="54"/>
+      <c r="G45" s="64" t="s">
         <v>124</v>
       </c>
       <c r="H45" s="31" t="s">
@@ -43072,12 +43069,12 @@
       <c r="A46" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B46" s="54"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="57"/>
-      <c r="G46" s="54"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="64"/>
       <c r="H46" s="25" t="s">
         <v>213</v>
       </c>
@@ -43137,18 +43134,18 @@
       <c r="A47" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B47" s="57"/>
-      <c r="C47" s="53" t="s">
+      <c r="B47" s="54"/>
+      <c r="C47" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="58" t="s">
+      <c r="D47" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="E47" s="56" t="s">
+      <c r="E47" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="F47" s="57"/>
-      <c r="G47" s="53" t="s">
+      <c r="F47" s="54"/>
+      <c r="G47" s="63" t="s">
         <v>128</v>
       </c>
       <c r="H47" s="31" t="s">
@@ -43210,12 +43207,12 @@
       <c r="A48" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B48" s="57"/>
-      <c r="C48" s="53"/>
-      <c r="D48" s="58"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="57"/>
-      <c r="G48" s="53"/>
+      <c r="B48" s="54"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="66"/>
+      <c r="E48" s="53"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="63"/>
       <c r="H48" s="25" t="s">
         <v>213</v>
       </c>
@@ -43275,20 +43272,20 @@
       <c r="A49" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="53" t="s">
+      <c r="C49" s="63" t="s">
         <v>131</v>
       </c>
-      <c r="D49" s="58" t="s">
+      <c r="D49" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="E49" s="53" t="s">
+      <c r="E49" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="F49" s="57"/>
-      <c r="G49" s="53" t="s">
+      <c r="F49" s="54"/>
+      <c r="G49" s="63" t="s">
         <v>134</v>
       </c>
       <c r="H49" s="31" t="s">
@@ -43307,28 +43304,28 @@
         <v>280</v>
       </c>
       <c r="M49" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="N49" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="O49" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="P49" s="34" t="s">
         <v>417</v>
       </c>
-      <c r="N49" s="35" t="s">
+      <c r="Q49" s="34" t="s">
         <v>418</v>
       </c>
-      <c r="O49" s="35" t="s">
+      <c r="R49" s="34" t="s">
         <v>418</v>
       </c>
-      <c r="P49" s="34" t="s">
+      <c r="S49" s="34" t="s">
         <v>419</v>
       </c>
-      <c r="Q49" s="34" t="s">
-        <v>420</v>
-      </c>
-      <c r="R49" s="34" t="s">
-        <v>420</v>
-      </c>
-      <c r="S49" s="34" t="s">
-        <v>421</v>
-      </c>
       <c r="T49" s="34" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="U49" s="5"/>
       <c r="V49" s="5"/>
@@ -43350,12 +43347,12 @@
       <c r="A50" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B50" s="56"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="53"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="66"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="63"/>
       <c r="H50" s="25" t="s">
         <v>249</v>
       </c>
@@ -43366,34 +43363,34 @@
         <v>249</v>
       </c>
       <c r="K50" s="25" t="s">
+        <v>420</v>
+      </c>
+      <c r="L50" s="25" t="s">
+        <v>421</v>
+      </c>
+      <c r="M50" s="33" t="s">
+        <v>557</v>
+      </c>
+      <c r="N50" s="33" t="s">
+        <v>557</v>
+      </c>
+      <c r="O50" s="33" t="s">
+        <v>557</v>
+      </c>
+      <c r="P50" s="33" t="s">
         <v>422</v>
       </c>
-      <c r="L50" s="25" t="s">
+      <c r="Q50" s="33" t="s">
+        <v>421</v>
+      </c>
+      <c r="R50" s="33" t="s">
+        <v>421</v>
+      </c>
+      <c r="S50" s="33" t="s">
         <v>423</v>
       </c>
-      <c r="M50" s="33" t="s">
-        <v>424</v>
-      </c>
-      <c r="N50" s="33" t="s">
-        <v>424</v>
-      </c>
-      <c r="O50" s="33" t="s">
-        <v>424</v>
-      </c>
-      <c r="P50" s="33" t="s">
-        <v>425</v>
-      </c>
-      <c r="Q50" s="33" t="s">
+      <c r="T50" s="33" t="s">
         <v>423</v>
-      </c>
-      <c r="R50" s="33" t="s">
-        <v>423</v>
-      </c>
-      <c r="S50" s="33" t="s">
-        <v>426</v>
-      </c>
-      <c r="T50" s="33" t="s">
-        <v>426</v>
       </c>
       <c r="U50" s="5"/>
       <c r="V50" s="5"/>
@@ -43415,20 +43412,20 @@
       <c r="A51" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B51" s="54" t="s">
+      <c r="B51" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C51" s="53" t="s">
+      <c r="C51" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="D51" s="55" t="s">
+      <c r="D51" s="65" t="s">
         <v>138</v>
       </c>
-      <c r="E51" s="56" t="s">
+      <c r="E51" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="F51" s="57"/>
-      <c r="G51" s="54" t="s">
+      <c r="F51" s="54"/>
+      <c r="G51" s="64" t="s">
         <v>140</v>
       </c>
       <c r="H51" s="31" t="s">
@@ -43441,28 +43438,28 @@
         <v>201</v>
       </c>
       <c r="K51" s="31" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="L51" s="31" t="s">
         <v>221</v>
       </c>
       <c r="M51" s="34" t="s">
+        <v>425</v>
+      </c>
+      <c r="N51" s="34" t="s">
+        <v>426</v>
+      </c>
+      <c r="O51" s="34" t="s">
+        <v>426</v>
+      </c>
+      <c r="P51" s="34" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q51" s="34" t="s">
         <v>428</v>
       </c>
-      <c r="N51" s="34" t="s">
-        <v>429</v>
-      </c>
-      <c r="O51" s="34" t="s">
-        <v>429</v>
-      </c>
-      <c r="P51" s="34" t="s">
-        <v>430</v>
-      </c>
-      <c r="Q51" s="34" t="s">
-        <v>431</v>
-      </c>
       <c r="R51" s="34" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="S51" s="34" t="s">
         <v>210</v>
@@ -43490,12 +43487,12 @@
       <c r="A52" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B52" s="54"/>
-      <c r="C52" s="53"/>
-      <c r="D52" s="55"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="57"/>
-      <c r="G52" s="54"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="63"/>
+      <c r="D52" s="65"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="64"/>
       <c r="H52" s="25" t="s">
         <v>213</v>
       </c>
@@ -43509,28 +43506,28 @@
         <v>215</v>
       </c>
       <c r="L52" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="M52" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="N52" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="O52" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="P52" s="33" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q52" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="R52" s="33" t="s">
+        <v>430</v>
+      </c>
+      <c r="S52" s="33" t="s">
         <v>432</v>
-      </c>
-      <c r="M52" s="33" t="s">
-        <v>433</v>
-      </c>
-      <c r="N52" s="33" t="s">
-        <v>433</v>
-      </c>
-      <c r="O52" s="33" t="s">
-        <v>433</v>
-      </c>
-      <c r="P52" s="33" t="s">
-        <v>434</v>
-      </c>
-      <c r="Q52" s="33" t="s">
-        <v>433</v>
-      </c>
-      <c r="R52" s="33" t="s">
-        <v>433</v>
-      </c>
-      <c r="S52" s="33" t="s">
-        <v>435</v>
       </c>
       <c r="T52" s="33" t="s">
         <v>219</v>
@@ -43555,20 +43552,20 @@
       <c r="A53" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B53" s="54" t="s">
+      <c r="B53" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="C53" s="53" t="s">
+      <c r="C53" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="D53" s="58" t="s">
+      <c r="D53" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="53" t="s">
+      <c r="E53" s="63" t="s">
         <v>142</v>
       </c>
-      <c r="F53" s="57"/>
-      <c r="G53" s="54" t="s">
+      <c r="F53" s="54"/>
+      <c r="G53" s="64" t="s">
         <v>143</v>
       </c>
       <c r="H53" s="31" t="s">
@@ -43581,7 +43578,7 @@
         <v>201</v>
       </c>
       <c r="K53" s="31" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="L53" s="31" t="s">
         <v>221</v>
@@ -43599,10 +43596,10 @@
         <v>208</v>
       </c>
       <c r="Q53" s="34" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="R53" s="34" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="S53" s="34" t="s">
         <v>210</v>
@@ -43630,12 +43627,12 @@
       <c r="A54" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B54" s="54"/>
-      <c r="C54" s="53"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="53"/>
-      <c r="F54" s="57"/>
-      <c r="G54" s="54"/>
+      <c r="B54" s="64"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="66"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="64"/>
       <c r="H54" s="25" t="s">
         <v>213</v>
       </c>
@@ -43649,28 +43646,28 @@
         <v>215</v>
       </c>
       <c r="L54" s="32" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="M54" s="33" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="N54" s="33" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="O54" s="33" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="P54" s="33" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="Q54" s="36" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="R54" s="36" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="S54" s="33" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="T54" s="33" t="s">
         <v>219</v>
@@ -43695,57 +43692,57 @@
       <c r="A55" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B55" s="56" t="s">
+      <c r="B55" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="53" t="s">
+      <c r="C55" s="63" t="s">
         <v>145</v>
       </c>
-      <c r="D55" s="58" t="s">
+      <c r="D55" s="66" t="s">
         <v>146</v>
       </c>
-      <c r="E55" s="53" t="s">
+      <c r="E55" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="F55" s="57"/>
-      <c r="G55" s="53" t="s">
+      <c r="F55" s="54"/>
+      <c r="G55" s="63" t="s">
         <v>148</v>
       </c>
       <c r="H55" s="31" t="s">
         <v>201</v>
       </c>
       <c r="I55" s="31" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="J55" s="31" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="K55" s="31" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="L55" s="31" t="s">
         <v>280</v>
       </c>
       <c r="M55" s="34" t="s">
+        <v>441</v>
+      </c>
+      <c r="N55" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="O55" s="35" t="s">
+        <v>442</v>
+      </c>
+      <c r="P55" s="34" t="s">
+        <v>443</v>
+      </c>
+      <c r="Q55" s="34" t="s">
         <v>444</v>
       </c>
-      <c r="N55" s="35" t="s">
+      <c r="R55" s="34" t="s">
+        <v>444</v>
+      </c>
+      <c r="S55" s="34" t="s">
         <v>445</v>
-      </c>
-      <c r="O55" s="35" t="s">
-        <v>445</v>
-      </c>
-      <c r="P55" s="34" t="s">
-        <v>446</v>
-      </c>
-      <c r="Q55" s="34" t="s">
-        <v>447</v>
-      </c>
-      <c r="R55" s="34" t="s">
-        <v>447</v>
-      </c>
-      <c r="S55" s="34" t="s">
-        <v>448</v>
       </c>
       <c r="T55" s="34" t="s">
         <v>211</v>
@@ -43770,12 +43767,12 @@
       <c r="A56" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B56" s="56"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="57"/>
-      <c r="G56" s="53"/>
+      <c r="B56" s="53"/>
+      <c r="C56" s="63"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="63"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="63"/>
       <c r="H56" s="25" t="s">
         <v>213</v>
       </c>
@@ -43786,31 +43783,31 @@
         <v>249</v>
       </c>
       <c r="K56" s="25" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L56" s="25" t="s">
         <v>288</v>
       </c>
       <c r="M56" s="33" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="N56" s="33" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="O56" s="33" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="P56" s="33" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="Q56" s="33" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="R56" s="33" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="S56" s="33" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="T56" s="33" t="s">
         <v>219</v>
@@ -43835,19 +43832,19 @@
       <c r="A57" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B57" s="57"/>
-      <c r="C57" s="53" t="s">
+      <c r="B57" s="54"/>
+      <c r="C57" s="63" t="s">
+        <v>534</v>
+      </c>
+      <c r="D57" s="66" t="s">
+        <v>535</v>
+      </c>
+      <c r="E57" s="53" t="s">
+        <v>538</v>
+      </c>
+      <c r="F57" s="54"/>
+      <c r="G57" s="63" t="s">
         <v>537</v>
-      </c>
-      <c r="D57" s="58" t="s">
-        <v>538</v>
-      </c>
-      <c r="E57" s="56" t="s">
-        <v>541</v>
-      </c>
-      <c r="F57" s="57"/>
-      <c r="G57" s="53" t="s">
-        <v>540</v>
       </c>
       <c r="H57" s="31"/>
       <c r="I57" s="31"/>
@@ -43882,37 +43879,37 @@
       <c r="A58" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B58" s="57"/>
-      <c r="C58" s="53"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="56"/>
-      <c r="F58" s="57"/>
-      <c r="G58" s="53"/>
+      <c r="B58" s="54"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="66"/>
+      <c r="E58" s="53"/>
+      <c r="F58" s="54"/>
+      <c r="G58" s="63"/>
       <c r="H58" s="25"/>
       <c r="I58" s="25"/>
       <c r="J58" s="25"/>
       <c r="K58" s="25"/>
       <c r="L58" s="25"/>
       <c r="M58" s="33" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="N58" s="33" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="O58" s="33" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="P58" s="33" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="Q58" s="33" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="R58" s="33" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="S58" s="33" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="T58" s="33" t="s">
         <v>219</v>
@@ -43937,58 +43934,58 @@
       <c r="A59" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B59" s="57"/>
-      <c r="C59" s="53" t="s">
+      <c r="B59" s="54"/>
+      <c r="C59" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D59" s="58" t="s">
+      <c r="D59" s="66" t="s">
         <v>151</v>
       </c>
-      <c r="E59" s="56" t="s">
+      <c r="E59" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="F59" s="57"/>
-      <c r="G59" s="53" t="s">
+      <c r="F59" s="54"/>
+      <c r="G59" s="63" t="s">
         <v>153</v>
       </c>
       <c r="H59" s="31" t="s">
         <v>252</v>
       </c>
       <c r="I59" s="31" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="J59" s="31" t="s">
         <v>252</v>
       </c>
       <c r="K59" s="31" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="L59" s="31" t="s">
         <v>204</v>
       </c>
       <c r="M59" s="34" t="s">
+        <v>452</v>
+      </c>
+      <c r="N59" s="34" t="s">
+        <v>453</v>
+      </c>
+      <c r="O59" s="34" t="s">
+        <v>453</v>
+      </c>
+      <c r="P59" s="34" t="s">
+        <v>454</v>
+      </c>
+      <c r="Q59" s="34" t="s">
         <v>455</v>
       </c>
-      <c r="N59" s="34" t="s">
+      <c r="R59" s="34" t="s">
+        <v>455</v>
+      </c>
+      <c r="S59" s="34" t="s">
         <v>456</v>
       </c>
-      <c r="O59" s="34" t="s">
+      <c r="T59" s="34" t="s">
         <v>456</v>
-      </c>
-      <c r="P59" s="34" t="s">
-        <v>457</v>
-      </c>
-      <c r="Q59" s="34" t="s">
-        <v>458</v>
-      </c>
-      <c r="R59" s="34" t="s">
-        <v>458</v>
-      </c>
-      <c r="S59" s="34" t="s">
-        <v>459</v>
-      </c>
-      <c r="T59" s="34" t="s">
-        <v>459</v>
       </c>
       <c r="U59" s="5"/>
       <c r="V59" s="5"/>
@@ -44010,12 +44007,12 @@
       <c r="A60" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B60" s="57"/>
-      <c r="C60" s="53"/>
-      <c r="D60" s="58"/>
-      <c r="E60" s="56"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="53"/>
+      <c r="B60" s="54"/>
+      <c r="C60" s="63"/>
+      <c r="D60" s="66"/>
+      <c r="E60" s="53"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="63"/>
       <c r="H60" s="25" t="s">
         <v>213</v>
       </c>
@@ -44029,7 +44026,7 @@
         <v>322</v>
       </c>
       <c r="L60" s="25" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="M60" s="33" t="s">
         <v>324</v>
@@ -44075,58 +44072,58 @@
       <c r="A61" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B61" s="57"/>
-      <c r="C61" s="53" t="s">
+      <c r="B61" s="54"/>
+      <c r="C61" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="D61" s="58" t="s">
+      <c r="D61" s="66" t="s">
         <v>155</v>
       </c>
-      <c r="E61" s="56" t="s">
+      <c r="E61" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="F61" s="57"/>
-      <c r="G61" s="53" t="s">
+      <c r="F61" s="54"/>
+      <c r="G61" s="63" t="s">
         <v>157</v>
       </c>
       <c r="H61" s="31" t="s">
         <v>268</v>
       </c>
       <c r="I61" s="31" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="J61" s="31" t="s">
         <v>268</v>
       </c>
       <c r="K61" s="31" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="L61" s="31" t="s">
         <v>204</v>
       </c>
       <c r="M61" s="34" t="s">
+        <v>459</v>
+      </c>
+      <c r="N61" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="O61" s="34" t="s">
+        <v>460</v>
+      </c>
+      <c r="P61" s="34" t="s">
+        <v>461</v>
+      </c>
+      <c r="Q61" s="34" t="s">
         <v>462</v>
       </c>
-      <c r="N61" s="34" t="s">
+      <c r="R61" s="34" t="s">
+        <v>462</v>
+      </c>
+      <c r="S61" s="34" t="s">
         <v>463</v>
       </c>
-      <c r="O61" s="34" t="s">
+      <c r="T61" s="34" t="s">
         <v>463</v>
-      </c>
-      <c r="P61" s="34" t="s">
-        <v>464</v>
-      </c>
-      <c r="Q61" s="34" t="s">
-        <v>465</v>
-      </c>
-      <c r="R61" s="34" t="s">
-        <v>465</v>
-      </c>
-      <c r="S61" s="34" t="s">
-        <v>466</v>
-      </c>
-      <c r="T61" s="34" t="s">
-        <v>466</v>
       </c>
       <c r="U61" s="5"/>
       <c r="V61" s="5"/>
@@ -44148,12 +44145,12 @@
       <c r="A62" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B62" s="57"/>
-      <c r="C62" s="53"/>
-      <c r="D62" s="58"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="57"/>
-      <c r="G62" s="53"/>
+      <c r="B62" s="54"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="54"/>
+      <c r="G62" s="63"/>
       <c r="H62" s="25" t="s">
         <v>213</v>
       </c>
@@ -44164,10 +44161,10 @@
         <v>213</v>
       </c>
       <c r="K62" s="25" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="L62" s="25" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="M62" s="33" t="s">
         <v>324</v>
@@ -44213,60 +44210,60 @@
       <c r="A63" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B63" s="56" t="s">
+      <c r="B63" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="53" t="s">
+      <c r="C63" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="D63" s="58" t="s">
+      <c r="D63" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="E63" s="56" t="s">
+      <c r="E63" s="53" t="s">
         <v>160</v>
       </c>
-      <c r="F63" s="57"/>
-      <c r="G63" s="53" t="s">
+      <c r="F63" s="54"/>
+      <c r="G63" s="63" t="s">
         <v>161</v>
       </c>
       <c r="H63" s="31" t="s">
+        <v>466</v>
+      </c>
+      <c r="I63" s="31" t="s">
+        <v>467</v>
+      </c>
+      <c r="J63" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="K63" s="31" t="s">
         <v>469</v>
-      </c>
-      <c r="I63" s="31" t="s">
-        <v>470</v>
-      </c>
-      <c r="J63" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="K63" s="31" t="s">
-        <v>472</v>
       </c>
       <c r="L63" s="31" t="s">
         <v>280</v>
       </c>
       <c r="M63" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="N63" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="O63" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="P63" s="34" t="s">
+        <v>471</v>
+      </c>
+      <c r="Q63" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="R63" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="S63" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="N63" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="O63" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="P63" s="34" t="s">
+      <c r="T63" s="34" t="s">
         <v>474</v>
-      </c>
-      <c r="Q63" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="R63" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="S63" s="34" t="s">
-        <v>476</v>
-      </c>
-      <c r="T63" s="34" t="s">
-        <v>477</v>
       </c>
       <c r="U63" s="5"/>
       <c r="V63" s="5"/>
@@ -44288,12 +44285,12 @@
       <c r="A64" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B64" s="56"/>
-      <c r="C64" s="53"/>
-      <c r="D64" s="58"/>
-      <c r="E64" s="56"/>
-      <c r="F64" s="57"/>
-      <c r="G64" s="53"/>
+      <c r="B64" s="53"/>
+      <c r="C64" s="63"/>
+      <c r="D64" s="66"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="54"/>
+      <c r="G64" s="63"/>
       <c r="H64" s="25" t="s">
         <v>249</v>
       </c>
@@ -44304,16 +44301,16 @@
         <v>249</v>
       </c>
       <c r="K64" s="25" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="L64" s="25" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="M64" s="33"/>
       <c r="N64" s="33"/>
       <c r="O64" s="33"/>
       <c r="P64" s="33" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="Q64" s="33"/>
       <c r="R64" s="33"/>
@@ -44339,60 +44336,60 @@
       <c r="A65" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B65" s="56" t="s">
+      <c r="B65" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C65" s="53" t="s">
+      <c r="C65" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="D65" s="58" t="s">
+      <c r="D65" s="66" t="s">
         <v>164</v>
       </c>
-      <c r="E65" s="56" t="s">
+      <c r="E65" s="53" t="s">
         <v>165</v>
       </c>
-      <c r="F65" s="57"/>
-      <c r="G65" s="53" t="s">
+      <c r="F65" s="54"/>
+      <c r="G65" s="63" t="s">
         <v>166</v>
       </c>
       <c r="H65" s="31" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I65" s="31" t="s">
+        <v>467</v>
+      </c>
+      <c r="J65" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="K65" s="31" t="s">
+        <v>477</v>
+      </c>
+      <c r="L65" s="31" t="s">
+        <v>478</v>
+      </c>
+      <c r="M65" s="34" t="s">
         <v>470</v>
       </c>
-      <c r="J65" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="K65" s="31" t="s">
-        <v>480</v>
-      </c>
-      <c r="L65" s="31" t="s">
-        <v>481</v>
-      </c>
-      <c r="M65" s="34" t="s">
+      <c r="N65" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="O65" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="P65" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q65" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="R65" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="S65" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="N65" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="O65" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="P65" s="34" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q65" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="R65" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="S65" s="34" t="s">
-        <v>476</v>
-      </c>
       <c r="T65" s="34" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="U65" s="5"/>
       <c r="V65" s="5"/>
@@ -44414,12 +44411,12 @@
       <c r="A66" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B66" s="56"/>
-      <c r="C66" s="53"/>
-      <c r="D66" s="58"/>
-      <c r="E66" s="56"/>
-      <c r="F66" s="57"/>
-      <c r="G66" s="53"/>
+      <c r="B66" s="53"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="66"/>
+      <c r="E66" s="53"/>
+      <c r="F66" s="54"/>
+      <c r="G66" s="63"/>
       <c r="H66" s="25" t="s">
         <v>249</v>
       </c>
@@ -44431,13 +44428,13 @@
       </c>
       <c r="K66" s="25"/>
       <c r="L66" s="25" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="M66" s="33"/>
       <c r="N66" s="33"/>
       <c r="O66" s="33"/>
       <c r="P66" s="33" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="Q66" s="33"/>
       <c r="R66" s="33"/>
@@ -44463,60 +44460,60 @@
       <c r="A67" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B67" s="56" t="s">
+      <c r="B67" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C67" s="53" t="s">
+      <c r="C67" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="D67" s="55" t="s">
+      <c r="D67" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="E67" s="53" t="s">
+      <c r="E67" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="F67" s="57"/>
-      <c r="G67" s="53" t="s">
+      <c r="F67" s="54"/>
+      <c r="G67" s="63" t="s">
         <v>171</v>
       </c>
       <c r="H67" s="31" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I67" s="31" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="J67" s="31" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="K67" s="31" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="L67" s="31" t="s">
         <v>280</v>
       </c>
       <c r="M67" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="N67" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="O67" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="P67" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q67" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="R67" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="S67" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="N67" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="O67" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="P67" s="34" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q67" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="R67" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="S67" s="34" t="s">
-        <v>476</v>
-      </c>
       <c r="T67" s="34" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="U67" s="5"/>
       <c r="V67" s="5"/>
@@ -44538,12 +44535,12 @@
       <c r="A68" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B68" s="56"/>
-      <c r="C68" s="53"/>
-      <c r="D68" s="55"/>
-      <c r="E68" s="53"/>
-      <c r="F68" s="57"/>
-      <c r="G68" s="53"/>
+      <c r="B68" s="53"/>
+      <c r="C68" s="63"/>
+      <c r="D68" s="65"/>
+      <c r="E68" s="63"/>
+      <c r="F68" s="54"/>
+      <c r="G68" s="63"/>
       <c r="H68" s="25" t="s">
         <v>249</v>
       </c>
@@ -44555,13 +44552,13 @@
       </c>
       <c r="K68" s="25"/>
       <c r="L68" s="25" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="M68" s="33"/>
       <c r="N68" s="33"/>
       <c r="O68" s="33"/>
       <c r="P68" s="33" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="Q68" s="33"/>
       <c r="R68" s="33"/>
@@ -44587,60 +44584,60 @@
       <c r="A69" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B69" s="56" t="s">
+      <c r="B69" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C69" s="53" t="s">
+      <c r="C69" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="D69" s="58" t="s">
+      <c r="D69" s="66" t="s">
         <v>173</v>
       </c>
-      <c r="E69" s="56" t="s">
+      <c r="E69" s="53" t="s">
         <v>174</v>
       </c>
-      <c r="F69" s="57"/>
-      <c r="G69" s="53" t="s">
+      <c r="F69" s="54"/>
+      <c r="G69" s="63" t="s">
         <v>175</v>
       </c>
       <c r="H69" s="31" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I69" s="31" t="s">
+        <v>467</v>
+      </c>
+      <c r="J69" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="K69" s="31" t="s">
+        <v>483</v>
+      </c>
+      <c r="L69" s="31" t="s">
+        <v>484</v>
+      </c>
+      <c r="M69" s="34" t="s">
         <v>470</v>
       </c>
-      <c r="J69" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="K69" s="31" t="s">
-        <v>486</v>
-      </c>
-      <c r="L69" s="31" t="s">
-        <v>487</v>
-      </c>
-      <c r="M69" s="34" t="s">
+      <c r="N69" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="O69" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="P69" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q69" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="R69" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="S69" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="N69" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="O69" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="P69" s="34" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q69" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="R69" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="S69" s="34" t="s">
-        <v>476</v>
-      </c>
       <c r="T69" s="34" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="U69" s="5"/>
       <c r="V69" s="5"/>
@@ -44662,12 +44659,12 @@
       <c r="A70" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B70" s="56"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="56"/>
-      <c r="F70" s="57"/>
-      <c r="G70" s="53"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="63"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="54"/>
+      <c r="G70" s="63"/>
       <c r="H70" s="25" t="s">
         <v>249</v>
       </c>
@@ -44679,13 +44676,13 @@
       </c>
       <c r="K70" s="25"/>
       <c r="L70" s="25" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="M70" s="33"/>
       <c r="N70" s="33"/>
       <c r="O70" s="33"/>
       <c r="P70" s="33" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="Q70" s="33"/>
       <c r="R70" s="33"/>
@@ -44711,60 +44708,60 @@
       <c r="A71" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B71" s="56" t="s">
+      <c r="B71" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C71" s="53" t="s">
+      <c r="C71" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="D71" s="58" t="s">
+      <c r="D71" s="66" t="s">
         <v>177</v>
       </c>
-      <c r="E71" s="56" t="s">
+      <c r="E71" s="53" t="s">
         <v>178</v>
       </c>
-      <c r="F71" s="57"/>
-      <c r="G71" s="53" t="s">
+      <c r="F71" s="54"/>
+      <c r="G71" s="63" t="s">
         <v>179</v>
       </c>
       <c r="H71" s="31" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I71" s="31" t="s">
+        <v>467</v>
+      </c>
+      <c r="J71" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="K71" s="31" t="s">
+        <v>486</v>
+      </c>
+      <c r="L71" s="31" t="s">
+        <v>487</v>
+      </c>
+      <c r="M71" s="34" t="s">
         <v>470</v>
       </c>
-      <c r="J71" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="K71" s="31" t="s">
+      <c r="N71" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="O71" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="P71" s="34" t="s">
+        <v>488</v>
+      </c>
+      <c r="Q71" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="R71" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="S71" s="34" t="s">
         <v>489</v>
       </c>
-      <c r="L71" s="31" t="s">
-        <v>490</v>
-      </c>
-      <c r="M71" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="N71" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="O71" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="P71" s="34" t="s">
-        <v>491</v>
-      </c>
-      <c r="Q71" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="R71" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="S71" s="34" t="s">
-        <v>492</v>
-      </c>
       <c r="T71" s="34" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="U71" s="5"/>
       <c r="V71" s="5"/>
@@ -44786,12 +44783,12 @@
       <c r="A72" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B72" s="56"/>
-      <c r="C72" s="53"/>
-      <c r="D72" s="58"/>
-      <c r="E72" s="56"/>
-      <c r="F72" s="57"/>
-      <c r="G72" s="53"/>
+      <c r="B72" s="53"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="66"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="54"/>
+      <c r="G72" s="63"/>
       <c r="H72" s="25" t="s">
         <v>249</v>
       </c>
@@ -44802,21 +44799,21 @@
         <v>249</v>
       </c>
       <c r="K72" s="25" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="L72" s="25" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="M72" s="33"/>
       <c r="N72" s="33"/>
       <c r="O72" s="33"/>
       <c r="P72" s="33" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="Q72" s="33"/>
       <c r="R72" s="33"/>
       <c r="S72" s="33" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="T72" s="33"/>
       <c r="U72" s="5"/>
@@ -44839,60 +44836,60 @@
       <c r="A73" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B73" s="56" t="s">
+      <c r="B73" s="53" t="s">
         <v>58</v>
       </c>
-      <c r="C73" s="53" t="s">
+      <c r="C73" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="D73" s="58" t="s">
+      <c r="D73" s="66" t="s">
         <v>183</v>
       </c>
-      <c r="E73" s="56" t="s">
+      <c r="E73" s="53" t="s">
         <v>184</v>
       </c>
-      <c r="F73" s="57"/>
-      <c r="G73" s="53" t="s">
+      <c r="F73" s="54"/>
+      <c r="G73" s="63" t="s">
         <v>185</v>
       </c>
       <c r="H73" s="31" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I73" s="31" t="s">
+        <v>467</v>
+      </c>
+      <c r="J73" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="K73" s="31" t="s">
+        <v>477</v>
+      </c>
+      <c r="L73" s="31" t="s">
+        <v>493</v>
+      </c>
+      <c r="M73" s="34" t="s">
         <v>470</v>
       </c>
-      <c r="J73" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="K73" s="31" t="s">
-        <v>480</v>
-      </c>
-      <c r="L73" s="31" t="s">
-        <v>496</v>
-      </c>
-      <c r="M73" s="34" t="s">
+      <c r="N73" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="O73" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="P73" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q73" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="R73" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="S73" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="N73" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="O73" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="P73" s="34" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q73" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="R73" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="S73" s="34" t="s">
-        <v>476</v>
-      </c>
       <c r="T73" s="34" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="U73" s="5"/>
       <c r="V73" s="5"/>
@@ -44914,12 +44911,12 @@
       <c r="A74" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B74" s="56"/>
-      <c r="C74" s="53"/>
-      <c r="D74" s="58"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="57"/>
-      <c r="G74" s="53"/>
+      <c r="B74" s="53"/>
+      <c r="C74" s="63"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="53"/>
+      <c r="F74" s="54"/>
+      <c r="G74" s="63"/>
       <c r="H74" s="25" t="s">
         <v>249</v>
       </c>
@@ -44931,13 +44928,13 @@
       </c>
       <c r="K74" s="25"/>
       <c r="L74" s="25" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="M74" s="37"/>
       <c r="N74" s="37"/>
       <c r="O74" s="37"/>
       <c r="P74" s="37" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="Q74" s="37"/>
       <c r="R74" s="37"/>
@@ -44963,60 +44960,60 @@
       <c r="A75" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B75" s="56" t="s">
+      <c r="B75" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C75" s="53" t="s">
+      <c r="C75" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="D75" s="58" t="s">
+      <c r="D75" s="66" t="s">
         <v>187</v>
       </c>
-      <c r="E75" s="56" t="s">
+      <c r="E75" s="53" t="s">
         <v>188</v>
       </c>
-      <c r="F75" s="57"/>
-      <c r="G75" s="53" t="s">
+      <c r="F75" s="54"/>
+      <c r="G75" s="63" t="s">
         <v>189</v>
       </c>
       <c r="H75" s="31" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I75" s="31" t="s">
+        <v>467</v>
+      </c>
+      <c r="J75" s="31" t="s">
+        <v>468</v>
+      </c>
+      <c r="K75" s="31" t="s">
+        <v>477</v>
+      </c>
+      <c r="L75" s="31" t="s">
+        <v>495</v>
+      </c>
+      <c r="M75" s="34" t="s">
         <v>470</v>
       </c>
-      <c r="J75" s="31" t="s">
-        <v>471</v>
-      </c>
-      <c r="K75" s="31" t="s">
-        <v>480</v>
-      </c>
-      <c r="L75" s="31" t="s">
-        <v>498</v>
-      </c>
-      <c r="M75" s="34" t="s">
+      <c r="N75" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="O75" s="34" t="s">
+        <v>470</v>
+      </c>
+      <c r="P75" s="34" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q75" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="R75" s="34" t="s">
+        <v>472</v>
+      </c>
+      <c r="S75" s="34" t="s">
         <v>473</v>
       </c>
-      <c r="N75" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="O75" s="34" t="s">
-        <v>473</v>
-      </c>
-      <c r="P75" s="34" t="s">
-        <v>482</v>
-      </c>
-      <c r="Q75" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="R75" s="34" t="s">
-        <v>475</v>
-      </c>
-      <c r="S75" s="34" t="s">
-        <v>476</v>
-      </c>
       <c r="T75" s="34" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="U75" s="5"/>
       <c r="V75" s="5"/>
@@ -45038,12 +45035,12 @@
       <c r="A76" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B76" s="56"/>
-      <c r="C76" s="53"/>
-      <c r="D76" s="58"/>
-      <c r="E76" s="56"/>
-      <c r="F76" s="57"/>
-      <c r="G76" s="53"/>
+      <c r="B76" s="53"/>
+      <c r="C76" s="63"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="53"/>
+      <c r="F76" s="54"/>
+      <c r="G76" s="63"/>
       <c r="H76" s="25" t="s">
         <v>249</v>
       </c>
@@ -45055,13 +45052,13 @@
       </c>
       <c r="K76" s="25"/>
       <c r="L76" s="25" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="M76" s="37"/>
       <c r="N76" s="37"/>
       <c r="O76" s="37"/>
       <c r="P76" s="37" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="Q76" s="37"/>
       <c r="R76" s="37"/>
@@ -45087,60 +45084,60 @@
       <c r="A77" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B77" s="56" t="s">
+      <c r="B77" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C77" s="53" t="s">
+      <c r="C77" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="D77" s="58" t="s">
+      <c r="D77" s="66" t="s">
         <v>190</v>
       </c>
-      <c r="E77" s="56" t="s">
+      <c r="E77" s="53" t="s">
         <v>191</v>
       </c>
-      <c r="F77" s="57"/>
-      <c r="G77" s="53" t="s">
+      <c r="F77" s="54"/>
+      <c r="G77" s="63" t="s">
         <v>192</v>
       </c>
       <c r="H77" s="31" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="I77" s="31" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="J77" s="31" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="K77" s="31" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="L77" s="31" t="s">
         <v>280</v>
       </c>
       <c r="M77" s="34" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="N77" s="34" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="O77" s="34" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="P77" s="34" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="Q77" s="34" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="R77" s="34" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="S77" s="34" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="T77" s="34" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="U77" s="5"/>
       <c r="V77" s="5"/>
@@ -45162,12 +45159,12 @@
       <c r="A78" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B78" s="56"/>
-      <c r="C78" s="53"/>
-      <c r="D78" s="58"/>
-      <c r="E78" s="56"/>
-      <c r="F78" s="57"/>
-      <c r="G78" s="53"/>
+      <c r="B78" s="53"/>
+      <c r="C78" s="63"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="53"/>
+      <c r="F78" s="54"/>
+      <c r="G78" s="63"/>
       <c r="H78" s="25" t="s">
         <v>249</v>
       </c>
@@ -45178,21 +45175,21 @@
         <v>249</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="L78" s="25" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="M78" s="33"/>
       <c r="N78" s="33"/>
       <c r="O78" s="33"/>
       <c r="P78" s="33" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="Q78" s="33"/>
       <c r="R78" s="33"/>
       <c r="S78" s="33" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="T78" s="33"/>
       <c r="U78" s="5"/>
@@ -45215,56 +45212,56 @@
       <c r="A79" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="B79" s="56" t="s">
+      <c r="B79" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="C79" s="53" t="s">
+      <c r="C79" s="63" t="s">
         <v>194</v>
       </c>
-      <c r="D79" s="58" t="s">
+      <c r="D79" s="66" t="s">
         <v>195</v>
       </c>
-      <c r="E79" s="56" t="s">
+      <c r="E79" s="53" t="s">
         <v>196</v>
       </c>
-      <c r="F79" s="57"/>
-      <c r="G79" s="53" t="s">
+      <c r="F79" s="54"/>
+      <c r="G79" s="63" t="s">
         <v>197</v>
       </c>
       <c r="H79" s="31"/>
       <c r="I79" s="31" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="J79" s="31"/>
       <c r="K79" s="31" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="L79" s="31" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="M79" s="34" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="N79" s="34" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="O79" s="34" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="P79" s="34" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="Q79" s="34" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="R79" s="34" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="S79" s="34" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="T79" s="34" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="U79" s="5"/>
       <c r="V79" s="5"/>
@@ -45286,12 +45283,12 @@
       <c r="A80" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B80" s="56"/>
-      <c r="C80" s="53"/>
-      <c r="D80" s="58"/>
-      <c r="E80" s="56"/>
-      <c r="F80" s="57"/>
-      <c r="G80" s="53"/>
+      <c r="B80" s="53"/>
+      <c r="C80" s="63"/>
+      <c r="D80" s="66"/>
+      <c r="E80" s="53"/>
+      <c r="F80" s="54"/>
+      <c r="G80" s="63"/>
       <c r="H80" s="25"/>
       <c r="I80" s="25" t="s">
         <v>249</v>
@@ -45299,18 +45296,18 @@
       <c r="J80" s="25"/>
       <c r="K80" s="25"/>
       <c r="L80" s="25" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="M80" s="33"/>
       <c r="N80" s="33"/>
       <c r="O80" s="33"/>
       <c r="P80" s="33" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="Q80" s="33"/>
       <c r="R80" s="33"/>
       <c r="S80" s="33" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="T80" s="33"/>
       <c r="U80" s="5"/>
@@ -68012,220 +68009,6 @@
     </row>
   </sheetData>
   <mergeCells count="238">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="G75:G76"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:G74"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="D9:D10"/>
@@ -68250,6 +68033,220 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="F63:F64"/>
+    <mergeCell ref="G63:G64"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="E67:E68"/>
+    <mergeCell ref="F67:F68"/>
+    <mergeCell ref="G67:G68"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="E65:E66"/>
+    <mergeCell ref="F65:F66"/>
+    <mergeCell ref="G65:G66"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="G73:G74"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -68273,19 +68270,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>506</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>507</v>
+      </c>
+      <c r="D1" s="47" t="s">
         <v>508</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="E1" s="47" t="s">
         <v>509</v>
-      </c>
-      <c r="C1" s="47" t="s">
-        <v>510</v>
-      </c>
-      <c r="D1" s="47" t="s">
-        <v>511</v>
-      </c>
-      <c r="E1" s="47" t="s">
-        <v>512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>